<commit_message>
added DataService, Filter Options
</commit_message>
<xml_diff>
--- a/Organisatorisches/Zeitenprotokoll.xlsx
+++ b/Organisatorisches/Zeitenprotokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CAEA69F1-CF1E-4649-8B2F-2558A031E086}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4AEB16A6-116E-4091-BA19-28D0BEFE7950}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{FD782830-D1B5-4D3B-9AF6-612AB898D10F}"/>
   </bookViews>
@@ -511,7 +511,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,14 +737,14 @@
         <v>43395</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16">
+    <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="2">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="3">
         <v>43402</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added pdf view for single round
</commit_message>
<xml_diff>
--- a/Organisatorisches/Zeitenprotokoll.xlsx
+++ b/Organisatorisches/Zeitenprotokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{97C40F33-EEA0-45BA-823C-C96CE98FC532}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B40417B5-C485-415C-9243-7E6A6E37FCD0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{FD782830-D1B5-4D3B-9AF6-612AB898D10F}"/>
   </bookViews>
@@ -511,7 +511,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,14 +770,14 @@
         <v>43402</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C19">
+    <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="2">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="3">
         <v>43402</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Tasks + Zeitenprotokoll
Minor changes at kv-translation
</commit_message>
<xml_diff>
--- a/Organisatorisches/Zeitenprotokoll.xlsx
+++ b/Organisatorisches/Zeitenprotokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{038B527E-45D6-4A58-B0A7-394BD30B931E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FA849259-201B-406D-81D8-DC3B98C9CAE8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{FD782830-D1B5-4D3B-9AF6-612AB898D10F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>User Story</t>
   </si>
@@ -150,13 +150,31 @@
     <t>CRUD-Tabelle anlegen</t>
   </si>
   <si>
-    <t>Drag &amp; Drop für Excel-Listen bzw. Bild</t>
-  </si>
-  <si>
     <t>Benutzerfreundliches Distance-Formular (123)</t>
   </si>
   <si>
     <t>Vergangene Ergebnisse (2015-2017) in Db einspeisen</t>
+  </si>
+  <si>
+    <t>Filtersuche nach Participant anlegen</t>
+  </si>
+  <si>
+    <t>Kontaktformular anlegen</t>
+  </si>
+  <si>
+    <t>Erweiterung der Clubergebnisse um Statistiktabellen</t>
+  </si>
+  <si>
+    <t>Website responsive machen</t>
+  </si>
+  <si>
+    <t>Email-Name Referenztabelle für Clubs erstellen</t>
+  </si>
+  <si>
+    <t>Suchfunktion nach einem Beweisbild</t>
+  </si>
+  <si>
+    <t>Website designen</t>
   </si>
 </sst>
 </file>
@@ -520,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29140236-DB94-4B4D-9C52-776B37635B80}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,7 +786,7 @@
         <v>33</v>
       </c>
       <c r="F17" s="1">
-        <v>43451</v>
+        <v>43465</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -793,26 +811,26 @@
         <v>43402</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="2">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="4">
         <v>7</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="5">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="2">
+        <v>8</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F21" s="3">
         <v>43402</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="4">
-        <v>8</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="5">
-        <v>43451</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -820,7 +838,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="3">
         <v>43451</v>
@@ -831,118 +849,190 @@
         <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F23" s="3">
         <v>43404</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>5</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C24" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="F24" s="3">
-        <v>43423</v>
-      </c>
-      <c r="G24" s="3">
-        <v>43451</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="2">
-        <v>2</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="3">
-        <v>43423</v>
+        <v>43446</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="4">
+        <v>12</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="5">
+        <v>43465</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="4">
+        <v>13</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="5">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="3">
+        <v>43423</v>
+      </c>
+      <c r="G27" s="3">
+        <v>43451</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="2">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="3">
+        <v>43423</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="4">
         <v>3</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="5">
-        <v>43451</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="1">
-        <v>43423</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>6</v>
-      </c>
-      <c r="B28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28" s="1">
-        <v>43451</v>
-      </c>
-      <c r="G28" s="1">
-        <v>43451</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="1">
-        <v>43455</v>
-      </c>
-      <c r="G29" s="1">
-        <v>43455</v>
+      <c r="F29" s="5">
+        <v>43465</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="5">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" s="5">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="5">
+        <v>43465</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C33">
         <v>2</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="5">
+        <v>43465</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="1">
-        <v>43455</v>
-      </c>
+      <c r="F34" s="5">
+        <v>43465</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="5">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="5">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F39" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>